<commit_message>
ci: update bsa form
</commit_message>
<xml_diff>
--- a/ONCHO/Breeding Site Survey/Cote d'Ivoire/2023/civ_oncho_bsa_3_result_202302.xlsx
+++ b/ONCHO/Breeding Site Survey/Cote d'Ivoire/2023/civ_oncho_bsa_3_result_202302.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\ONCHO\Breeding Site Survey\Cote d'Ivoire\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF89A7C-4198-4101-99DC-5F0CE9B39ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC212C7-A50F-4F91-873E-73DB054CCA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -7662,12 +7662,6 @@
     <t>district = ${d_district}</t>
   </si>
   <si>
-    <t>civ_oncho_bsa_3_result_202302_v2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2023 Fev) 3. Formulaire d’enregistrement des résultats V2 </t>
-  </si>
-  <si>
     <t>1. Entrer l'identifiant de l'enregistreur</t>
   </si>
   <si>
@@ -7698,7 +7692,13 @@
     <t>9. Présence de larves?</t>
   </si>
   <si>
-    <t>${d_presence_site} = 'Non'</t>
+    <t>${d_presence_site} = 'Oui'</t>
+  </si>
+  <si>
+    <t>(2023 Fev) 3. Formulaire d’enregistrement des résultats V2.1</t>
+  </si>
+  <si>
+    <t>civ_oncho_bsa_3_result_202302_v_12</t>
   </si>
 </sst>
 </file>
@@ -8128,11 +8128,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -8203,7 +8203,7 @@
         <v>192</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>15</v>
@@ -8231,7 +8231,7 @@
         <v>193</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>2549</v>
+        <v>2547</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -8252,7 +8252,7 @@
         <v>194</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>2550</v>
+        <v>2548</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -8275,7 +8275,7 @@
         <v>196</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>2551</v>
+        <v>2549</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -8299,7 +8299,7 @@
         <v>197</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>2554</v>
+        <v>2552</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>22</v>
@@ -8323,7 +8323,7 @@
         <v>198</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -8345,7 +8345,7 @@
         <v>199</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>2555</v>
+        <v>2553</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -8367,7 +8367,7 @@
         <v>200</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>2556</v>
+        <v>2554</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -8389,7 +8389,7 @@
         <v>201</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -8408,14 +8408,14 @@
         <v>205</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>2553</v>
+        <v>2551</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
       <c r="I11" s="9"/>
       <c r="L11" s="7"/>
@@ -44275,8 +44275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -44301,10 +44301,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
-        <v>2547</v>
+        <v>2557</v>
       </c>
       <c r="B2" t="s">
-        <v>2546</v>
+        <v>2558</v>
       </c>
       <c r="C2" t="s">
         <v>166</v>

</xml_diff>